<commit_message>
Import Customer - Supplier
</commit_message>
<xml_diff>
--- a/database/seeds/2020-06-18 data test/ยอดเจ้าหนี้  12-6.xlsx
+++ b/database/seeds/2020-06-18 data test/ยอดเจ้าหนี้  12-6.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kantachai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\megatech\database\seeds\2020-06-18 data test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EFEF9BE-4F06-49D4-8D3E-30D65EAF2AE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF0A81D-CF50-4CCF-A483-BEC3F02EA16B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E3EF150-887C-4B1D-98D6-F4A315230BB1}"/>
+    <workbookView minimized="1" xWindow="8730" yWindow="930" windowWidth="21600" windowHeight="11385" xr2:uid="{2E3EF150-887C-4B1D-98D6-F4A315230BB1}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>ACCID</t>
   </si>
@@ -94,6 +96,33 @@
   </si>
   <si>
     <t>บริษัท ทรูเทค แมชชินเนอรี่ จำกัด</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>XP</t>
+  </si>
+  <si>
+    <t>INSERT INTO supplier_debts (reference,total,doc_no,type_debt) VALUES (</t>
   </si>
 </sst>
 </file>
@@ -101,9 +130,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;฿&quot;* #,##0.00_-;\-&quot;฿&quot;* #,##0.00_-;_-&quot;฿&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;฿&quot;* #,##0.00_-;\-&quot;฿&quot;* #,##0.00_-;_-&quot;฿&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +156,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,18 +183,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
-    <cellStyle name="สกุลเงิน" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -174,7 +211,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -470,22 +507,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720DF2D2-6C03-415C-B245-E5692A5EE369}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -518,8 +559,33 @@
       <c r="E2" s="3">
         <v>1428463.91</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="str">
+        <f>"'"&amp;A2&amp;"',"</f>
+        <v>'DF0002',</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="L2:Q2" si="0">"'"&amp;E2&amp;"',"</f>
+        <v>'1428463.91',</v>
+      </c>
+      <c r="P2" t="str">
+        <f>"'"&amp;G2&amp;"2006-000"&amp;F2&amp;"',"</f>
+        <v>'XP2006-00001',</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>"'"&amp;G2&amp;"');"</f>
+        <v>'XP');</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -535,8 +601,33 @@
       <c r="E3" s="3">
         <v>75626.53</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K8" si="1">"'"&amp;A3&amp;"',"</f>
+        <v>'DI0001',</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O8" si="2">"'"&amp;E3&amp;"',"</f>
+        <v>'75626.53',</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P8" si="3">"'"&amp;G3&amp;"2006-000"&amp;F3&amp;"',"</f>
+        <v>'XP2006-00002',</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q8" si="4">"'"&amp;G3&amp;"');"</f>
+        <v>'XP');</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:17">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -552,8 +643,33 @@
       <c r="E4" s="3">
         <v>9549.75</v>
       </c>
+      <c r="F4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>'DI0004*',</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="2"/>
+        <v>'9549.75',</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="3"/>
+        <v>'XP2006-00003',</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="4"/>
+        <v>'XP');</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:17">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -569,8 +685,33 @@
       <c r="E5" s="3">
         <v>24545.8</v>
       </c>
+      <c r="F5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>'DK0001',</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="2"/>
+        <v>'24545.8',</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="3"/>
+        <v>'XP2006-00004',</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="4"/>
+        <v>'XP');</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -586,8 +727,33 @@
       <c r="E6" s="3">
         <v>492258.85</v>
       </c>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>'DS0001',</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="2"/>
+        <v>'492258.85',</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="3"/>
+        <v>'XP2006-00005',</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="4"/>
+        <v>'XP');</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:17">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -603,8 +769,33 @@
       <c r="E7" s="3">
         <v>4085.26</v>
       </c>
+      <c r="F7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>'DS0006',</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="2"/>
+        <v>'4085.26',</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="3"/>
+        <v>'XP2006-00006',</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="4"/>
+        <v>'XP');</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:17">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -620,8 +811,34 @@
       <c r="E8" s="3">
         <v>6885.45</v>
       </c>
+      <c r="F8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>'DT0002',</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="2"/>
+        <v>'6885.45',</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="3"/>
+        <v>'XP2006-00007',</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="4"/>
+        <v>'XP');</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>